<commit_message>
Update importUser fuction and add fake data
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/User-Template.xlsx
+++ b/src/main/resources/templates/User-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023_Spring_OJT\fa-training-system\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049608C-8684-481C-9CEC-AB7B7180DB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CF09D5-B7E6-4EA6-BDE9-BB100CD205D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDEA2597-098A-4345-9CD1-EF6EED3D88B0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Full Name</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>image.com</t>
+  </si>
+  <si>
+    <t>12345</t>
   </si>
 </sst>
 </file>
@@ -139,13 +142,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,88 +468,90 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="4" width="13.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" style="3" customWidth="1"/>
+    <col min="3" max="4" width="13.21875" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
     <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="13.21875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <f>DATE(2002,2,20)</f>
         <v>37307</v>
       </c>

</xml_diff>

<commit_message>
Update export user to excel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/User-Template.xlsx
+++ b/src/main/resources/templates/User-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2023_Spring_OJT\fa-training-system\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CF09D5-B7E6-4EA6-BDE9-BB100CD205D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F74E99-BCE8-4D73-887F-0A4014765640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BDEA2597-098A-4345-9CD1-EF6EED3D88B0}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>